<commit_message>
Vraiment fonctionnel cette fois
</commit_message>
<xml_diff>
--- a/Code Opti Tournees Touristiques + Donnees-20240315/Resultats.xlsx
+++ b/Code Opti Tournees Touristiques + Donnees-20240315/Resultats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kergosien/Desktop/Cours Optim Discret/Conception itineraire Touristique/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Polytech\DI4\S8\Optimistion-Discrete\Code Opti Tournees Touristiques + Donnees-20240315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CFAA1F-C96E-204A-BF63-E71960990D9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3B1A78-5361-401E-AB19-BC66ED9F9A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{EA066B61-4340-A149-91F1-F19407D7865E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA066B61-4340-A149-91F1-F19407D7865E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Inst1</t>
   </si>
@@ -154,13 +154,16 @@
   </si>
   <si>
     <t>INSTANCES NON DISPONIBLES</t>
+  </si>
+  <si>
+    <t>Notre solution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,9 +221,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +261,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -364,7 +367,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -506,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,20 +517,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54003879-A489-2749-B9F8-7E0F21DD826C}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -536,7 +539,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -552,8 +555,11 @@
       <c r="E2" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -569,8 +575,11 @@
       <c r="E3">
         <v>816</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -586,8 +595,11 @@
       <c r="E4">
         <v>900</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -603,8 +615,11 @@
       <c r="E5">
         <v>1062</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -620,8 +635,11 @@
       <c r="E6">
         <v>1062</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -637,8 +655,11 @@
       <c r="E7">
         <v>1116</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -654,8 +675,11 @@
       <c r="E8">
         <v>1236</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -671,8 +695,11 @@
       <c r="E9">
         <v>1236</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -688,8 +715,11 @@
       <c r="E10">
         <v>1236</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -705,8 +735,11 @@
       <c r="E11">
         <v>1284</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -722,8 +755,11 @@
       <c r="E12">
         <v>1284</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="G12">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -739,8 +775,11 @@
       <c r="E13">
         <v>1284</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -756,8 +795,11 @@
       <c r="E14">
         <v>1670</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -773,8 +815,11 @@
       <c r="E15">
         <v>173</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -790,8 +835,11 @@
       <c r="E16">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -807,8 +855,11 @@
       <c r="E17">
         <v>367</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -824,8 +875,11 @@
       <c r="E18">
         <v>412</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -841,8 +895,11 @@
       <c r="E19">
         <v>412</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -858,8 +915,11 @@
       <c r="E20">
         <v>504</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -875,8 +935,11 @@
       <c r="E21">
         <v>504</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -892,8 +955,11 @@
       <c r="E22">
         <v>504</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -909,8 +975,11 @@
       <c r="E23">
         <v>590</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -926,8 +995,11 @@
       <c r="E24">
         <v>1114</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -943,8 +1015,11 @@
       <c r="E25">
         <v>1164</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -960,8 +1035,11 @@
       <c r="E26">
         <v>1234</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="G26">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -977,8 +1055,11 @@
       <c r="E27">
         <v>1234</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="G27">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -994,8 +1075,11 @@
       <c r="E28">
         <v>1261</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1011,8 +1095,11 @@
       <c r="E29">
         <v>1306</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="G29">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1021,7 +1108,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1038,7 +1125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1055,7 +1142,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1072,7 +1159,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1089,7 +1176,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1106,7 +1193,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1123,7 +1210,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1140,7 +1227,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1157,7 +1244,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -1174,7 +1261,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Resolutions de plusieurs problemes sur la metaheuristique
</commit_message>
<xml_diff>
--- a/Code Opti Tournees Touristiques + Donnees-20240315/Resultats.xlsx
+++ b/Code Opti Tournees Touristiques + Donnees-20240315/Resultats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Polytech\DI4\S8\Optimistion-Discrete\Code Opti Tournees Touristiques + Donnees-20240315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3B1A78-5361-401E-AB19-BC66ED9F9A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1738386-F9CF-476A-B583-8E5324628BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA066B61-4340-A149-91F1-F19407D7865E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA066B61-4340-A149-91F1-F19407D7865E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Inst1</t>
   </si>
@@ -156,7 +156,10 @@
     <t>INSTANCES NON DISPONIBLES</t>
   </si>
   <si>
-    <t>Notre solution</t>
+    <t>Notre Heuristique</t>
+  </si>
+  <si>
+    <t>Notre MetaHeuristique</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54003879-A489-2749-B9F8-7E0F21DD826C}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -530,7 +533,7 @@
     <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -539,7 +542,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -558,8 +561,11 @@
       <c r="G2" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -576,10 +582,13 @@
         <v>816</v>
       </c>
       <c r="G3">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+      <c r="I3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -596,10 +605,13 @@
         <v>900</v>
       </c>
       <c r="G4">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>786</v>
+      </c>
+      <c r="I4">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -618,8 +630,11 @@
       <c r="G5">
         <v>732</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -636,10 +651,13 @@
         <v>1062</v>
       </c>
       <c r="G6">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="I6">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -656,10 +674,13 @@
         <v>1116</v>
       </c>
       <c r="G7">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>756</v>
+      </c>
+      <c r="I7">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -676,10 +697,13 @@
         <v>1236</v>
       </c>
       <c r="G8">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+      <c r="I8">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -696,10 +720,13 @@
         <v>1236</v>
       </c>
       <c r="G9">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+      <c r="I9">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -716,10 +743,13 @@
         <v>1236</v>
       </c>
       <c r="G10">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>528</v>
+      </c>
+      <c r="I10">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -736,10 +766,13 @@
         <v>1284</v>
       </c>
       <c r="G11">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="I11">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -756,10 +789,13 @@
         <v>1284</v>
       </c>
       <c r="G12">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>726</v>
+      </c>
+      <c r="I12">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -776,10 +812,13 @@
         <v>1284</v>
       </c>
       <c r="G13">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="I13">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -796,10 +835,13 @@
         <v>1670</v>
       </c>
       <c r="G14">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>840</v>
+      </c>
+      <c r="I14">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -816,10 +858,13 @@
         <v>173</v>
       </c>
       <c r="G15">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="I15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -836,10 +881,13 @@
         <v>241</v>
       </c>
       <c r="G16">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="I16">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -856,10 +904,13 @@
         <v>367</v>
       </c>
       <c r="G17">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="I17">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -876,10 +927,13 @@
         <v>412</v>
       </c>
       <c r="G18">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+      <c r="I18">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -896,10 +950,13 @@
         <v>412</v>
       </c>
       <c r="G19">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="I19">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -916,10 +973,13 @@
         <v>504</v>
       </c>
       <c r="G20">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+      <c r="I20">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -936,10 +996,13 @@
         <v>504</v>
       </c>
       <c r="G21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+      <c r="I21">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -956,10 +1019,13 @@
         <v>504</v>
       </c>
       <c r="G22">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="I22">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -976,10 +1042,13 @@
         <v>590</v>
       </c>
       <c r="G23">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+      <c r="I23">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -996,10 +1065,13 @@
         <v>1114</v>
       </c>
       <c r="G24">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="I24">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1016,10 +1088,13 @@
         <v>1164</v>
       </c>
       <c r="G25">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+      <c r="I25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1036,10 +1111,13 @@
         <v>1234</v>
       </c>
       <c r="G26">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+      <c r="I26">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1056,10 +1134,13 @@
         <v>1234</v>
       </c>
       <c r="G27">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>624</v>
+      </c>
+      <c r="I27">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1076,10 +1157,13 @@
         <v>1261</v>
       </c>
       <c r="G28">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="I28">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1096,10 +1180,13 @@
         <v>1306</v>
       </c>
       <c r="G29">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>631</v>
+      </c>
+      <c r="I29">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1108,7 +1195,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Heuristique mise en forme
</commit_message>
<xml_diff>
--- a/Code Opti Tournees Touristiques + Donnees-20240315/Resultats.xlsx
+++ b/Code Opti Tournees Touristiques + Donnees-20240315/Resultats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Polytech\DI4\S8\Optimistion-Discrete\Code Opti Tournees Touristiques + Donnees-20240315\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57503A1-4922-488C-A32C-DF452A570821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706D94F5-38F9-4A3F-BDCD-CCA4422FA5FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EA066B61-4340-A149-91F1-F19407D7865E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA066B61-4340-A149-91F1-F19407D7865E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
     <t>Notre MetaHeuristique</t>
   </si>
   <si>
-    <t>Heuristique v2</t>
+    <t>Heuristique v3</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -613,9 +613,6 @@
         <v>900</v>
       </c>
       <c r="G4">
-        <v>786</v>
-      </c>
-      <c r="H4">
         <v>798</v>
       </c>
       <c r="I4">
@@ -639,9 +636,6 @@
         <v>1062</v>
       </c>
       <c r="G5">
-        <v>732</v>
-      </c>
-      <c r="H5">
         <v>810</v>
       </c>
       <c r="I5">
@@ -665,9 +659,6 @@
         <v>1062</v>
       </c>
       <c r="G6">
-        <v>300</v>
-      </c>
-      <c r="H6">
         <v>432</v>
       </c>
       <c r="I6">
@@ -691,9 +682,6 @@
         <v>1116</v>
       </c>
       <c r="G7">
-        <v>756</v>
-      </c>
-      <c r="H7">
         <v>816</v>
       </c>
       <c r="I7">
@@ -717,9 +705,6 @@
         <v>1236</v>
       </c>
       <c r="G8">
-        <v>522</v>
-      </c>
-      <c r="H8">
         <v>540</v>
       </c>
       <c r="I8">
@@ -743,9 +728,6 @@
         <v>1236</v>
       </c>
       <c r="G9">
-        <v>396</v>
-      </c>
-      <c r="H9">
         <v>492</v>
       </c>
       <c r="I9">
@@ -769,9 +751,6 @@
         <v>1236</v>
       </c>
       <c r="G10">
-        <v>528</v>
-      </c>
-      <c r="H10">
         <v>570</v>
       </c>
       <c r="I10">
@@ -795,9 +774,6 @@
         <v>1284</v>
       </c>
       <c r="G11">
-        <v>348</v>
-      </c>
-      <c r="H11">
         <v>414</v>
       </c>
       <c r="I11">
@@ -821,9 +797,6 @@
         <v>1284</v>
       </c>
       <c r="G12">
-        <v>726</v>
-      </c>
-      <c r="H12">
         <v>750</v>
       </c>
       <c r="I12">
@@ -847,9 +820,6 @@
         <v>1284</v>
       </c>
       <c r="G13">
-        <v>300</v>
-      </c>
-      <c r="H13">
         <v>318</v>
       </c>
       <c r="I13">
@@ -873,9 +843,6 @@
         <v>1670</v>
       </c>
       <c r="G14">
-        <v>840</v>
-      </c>
-      <c r="H14">
         <v>590</v>
       </c>
       <c r="I14">
@@ -945,9 +912,6 @@
         <v>367</v>
       </c>
       <c r="G17">
-        <v>229</v>
-      </c>
-      <c r="H17">
         <v>367</v>
       </c>
       <c r="I17">
@@ -971,9 +935,6 @@
         <v>412</v>
       </c>
       <c r="G18">
-        <v>378</v>
-      </c>
-      <c r="H18">
         <v>385</v>
       </c>
       <c r="I18">
@@ -1043,9 +1004,6 @@
         <v>504</v>
       </c>
       <c r="G21">
-        <v>404</v>
-      </c>
-      <c r="H21">
         <v>338</v>
       </c>
       <c r="I21">
@@ -1069,9 +1027,6 @@
         <v>504</v>
       </c>
       <c r="G22">
-        <v>398</v>
-      </c>
-      <c r="H22">
         <v>257</v>
       </c>
       <c r="I22">
@@ -1095,9 +1050,6 @@
         <v>590</v>
       </c>
       <c r="G23">
-        <v>345</v>
-      </c>
-      <c r="H23">
         <v>311</v>
       </c>
       <c r="I23">
@@ -1121,9 +1073,6 @@
         <v>1114</v>
       </c>
       <c r="G24">
-        <v>206</v>
-      </c>
-      <c r="H24">
         <v>256</v>
       </c>
       <c r="I24">
@@ -1147,9 +1096,6 @@
         <v>1164</v>
       </c>
       <c r="G25">
-        <v>642</v>
-      </c>
-      <c r="H25">
         <v>264</v>
       </c>
       <c r="I25">
@@ -1173,9 +1119,6 @@
         <v>1234</v>
       </c>
       <c r="G26">
-        <v>585</v>
-      </c>
-      <c r="H26">
         <v>466</v>
       </c>
       <c r="I26">
@@ -1199,9 +1142,6 @@
         <v>1234</v>
       </c>
       <c r="G27">
-        <v>624</v>
-      </c>
-      <c r="H27">
         <v>260</v>
       </c>
       <c r="I27">
@@ -1225,9 +1165,6 @@
         <v>1261</v>
       </c>
       <c r="G28">
-        <v>543</v>
-      </c>
-      <c r="H28">
         <v>178</v>
       </c>
       <c r="I28">
@@ -1251,9 +1188,6 @@
         <v>1306</v>
       </c>
       <c r="G29">
-        <v>631</v>
-      </c>
-      <c r="H29">
         <v>720</v>
       </c>
       <c r="I29">

</xml_diff>